<commit_message>
Adding logic to fetch column names from excel file and identify columns with URL
</commit_message>
<xml_diff>
--- a/sheet/test-urls.xlsx
+++ b/sheet/test-urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pawanjaiswal/Documents/Learning/repos/url-validator/sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D258E0D-D3A9-EC44-8C25-672EC8B65A23}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFABA61E-70D7-6C4E-B456-2F602B0D1B92}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13960" xr2:uid="{0BCB89F1-12A3-AB4A-A0C3-B58EFD1B922A}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding logic to test URL connectivity from the excel column
</commit_message>
<xml_diff>
--- a/sheet/test-urls.xlsx
+++ b/sheet/test-urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pawanjaiswal/Documents/Learning/repos/url-validator/sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFABA61E-70D7-6C4E-B456-2F602B0D1B92}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95A738F-1ACB-A640-8703-4D59448E2D34}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13960" xr2:uid="{0BCB89F1-12A3-AB4A-A0C3-B58EFD1B922A}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding logic to update the connection status in data frame
</commit_message>
<xml_diff>
--- a/sheet/test-urls.xlsx
+++ b/sheet/test-urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pawanjaiswal/Documents/Learning/repos/url-validator/sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95A738F-1ACB-A640-8703-4D59448E2D34}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8967006-5D6C-0E41-B0C2-7569936D6261}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13960" xr2:uid="{0BCB89F1-12A3-AB4A-A0C3-B58EFD1B922A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -36,9 +36,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Yahoo</t>
   </si>
   <si>
@@ -51,10 +48,10 @@
     <t>https://www.yahoo.com</t>
   </si>
   <si>
-    <t>https://www.google.com/?client=safari</t>
-  </si>
-  <si>
     <t>https://www.bing.com</t>
+  </si>
+  <si>
+    <t>google.com</t>
   </si>
 </sst>
 </file>
@@ -417,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D23E10E-D849-1447-A458-7E58A53D3472}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,7 +425,7 @@
     <col min="3" max="3" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,47 +435,44 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E978751D-871A-674D-B00E-CD6043F5177E}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{EE4535F7-7BED-C34C-AAD1-A95C19CEFF49}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://www.google.com/?client=safari" xr:uid="{EE4535F7-7BED-C34C-AAD1-A95C19CEFF49}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{D5E36761-2B5C-EE45-BB75-17103468D440}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to store connection status in the Excel file
</commit_message>
<xml_diff>
--- a/sheet/test-urls.xlsx
+++ b/sheet/test-urls.xlsx
@@ -1,89 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pawanjaiswal/Documents/Learning/repos/url-validator/sheet/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8967006-5D6C-0E41-B0C2-7569936D6261}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13960" xr2:uid="{0BCB89F1-12A3-AB4A-A0C3-B58EFD1B922A}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="URL Status" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Sr. No.</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Yahoo</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>Bing</t>
-  </si>
-  <si>
-    <t>https://www.yahoo.com</t>
-  </si>
-  <si>
-    <t>https://www.bing.com</t>
-  </si>
-  <si>
-    <t>google.com</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -91,29 +58,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,68 +466,227 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D23E10E-D849-1447-A458-7E58A53D3472}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col width="34.6640625" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Sr. No.</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>https://www.yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>google.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bing</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>https://www.bing.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E978751D-871A-674D-B00E-CD6043F5177E}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://www.google.com/?client=safari" xr:uid="{EE4535F7-7BED-C34C-AAD1-A95C19CEFF49}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{D5E36761-2B5C-EE45-BB75-17103468D440}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" display="https://www.google.com/?client=safari" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Sr. No.</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Yahoo</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.yahoo.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>google.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bing</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.bing.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>